<commit_message>
transition in docs and proj
</commit_message>
<xml_diff>
--- a/docs/FINAL_TABEL_TRANSISI.xlsx
+++ b/docs/FINAL_TABEL_TRANSISI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="64">
   <si>
     <t>State</t>
   </si>
@@ -133,13 +133,88 @@
   </si>
   <si>
     <t>Total State</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Dq9</t>
+  </si>
+  <si>
+    <t>Alias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,16 +228,65 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -199,11 +323,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -211,6 +452,98 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -586,7 +919,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>14</v>
@@ -662,7 +995,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
@@ -710,16 +1043,16 @@
       <c r="G7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="36" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="6" t="s">
@@ -742,23 +1075,23 @@
       <c r="G8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="38" t="s">
         <v>10</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
@@ -774,16 +1107,16 @@
       <c r="G9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="41" t="s">
         <v>10</v>
       </c>
       <c r="L9" s="6" t="s">
@@ -1193,7 +1526,7 @@
       <c r="E22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="21" t="s">
         <v>33</v>
       </c>
       <c r="G22" s="6" t="s">
@@ -1225,7 +1558,7 @@
       <c r="E23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="21" t="s">
         <v>30</v>
       </c>
       <c r="G23" s="6" t="s">
@@ -1260,7 +1593,7 @@
       <c r="F24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H24" s="6" t="s">
@@ -1292,7 +1625,7 @@
       <c r="F25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H25" s="6" t="s">
@@ -1324,7 +1657,7 @@
       <c r="F26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H26" s="6" t="s">
@@ -1356,7 +1689,7 @@
       <c r="F27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H27" s="6" t="s">
@@ -1388,7 +1721,7 @@
       <c r="F28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="22" t="s">
         <v>15</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -1424,13 +1757,988 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C17" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C18" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C19" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C20" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C21" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C22" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C23" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C24" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C25" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C27" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C28" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="1">
+        <f>COUNTA(C3:C28)-COUNTA(B10:B12)</f>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>